<commit_message>
Corrección correo almacén y actualización de Certificados no válidos DEV
</commit_message>
<xml_diff>
--- a/storage/app/templates/TRASLADO_ELEMENTOS.xlsx
+++ b/storage/app/templates/TRASLADO_ELEMENTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielprado/Sites/dashboard/storage/app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4256E9-6906-C44D-9C75-8CF89591CBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E254151-0050-654B-82BD-057A78D87BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>solicitudes.almacen@idrd.gov.co</t>
+      <t>almacen.solicitudes@idrd.gov.co</t>
     </r>
     <r>
       <rPr>
@@ -531,6 +531,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,6 +548,78 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -583,80 +663,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -665,12 +671,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1147,7 @@
   <dimension ref="B8:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="B10" sqref="B10:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,260 +1159,260 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1454,88 +1454,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="29"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="30"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="30"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="30"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
@@ -1553,199 +1553,199 @@
         <v>4</v>
       </c>
       <c r="M5" s="7"/>
-      <c r="N5" s="30"/>
+      <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="30"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="3"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="3"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="30"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="30"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="30"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="30"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="30"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="30"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="30"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="28"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
@@ -1777,6 +1777,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F13:M13"/>
+    <mergeCell ref="F14:M14"/>
+    <mergeCell ref="H15:M15"/>
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="N1:N15"/>
     <mergeCell ref="B3:D3"/>
@@ -1793,9 +1796,6 @@
     <mergeCell ref="B9:M12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F13:M13"/>
-    <mergeCell ref="F14:M14"/>
-    <mergeCell ref="H15:M15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup scale="71" orientation="landscape" r:id="rId1"/>

</xml_diff>